<commit_message>
All functionality except iterator completed
</commit_message>
<xml_diff>
--- a/6012/Uploaded Worksheets/assignmentArchive/assignment04 RawData.xlsx
+++ b/6012/Uploaded Worksheets/assignmentArchive/assignment04 RawData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epoole/Box Sync/erikpoole/6012/Uploaded Worksheets/assignmentArchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC1660E-7B25-4B43-BE02-07F0B27C9FC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6689820A-B7CE-B044-A136-FD86037AC3B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="28040" windowHeight="15660" xr2:uid="{E07FD9B9-E6D7-B844-A7A2-A761D0372312}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -122,10 +122,10 @@
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -2404,7 +2404,7 @@
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2459,7 +2459,7 @@
         <v>1.7408E-2</v>
       </c>
       <c r="F2" s="10">
-        <f t="shared" ref="F2:F12" si="1">1.6*(A2*LOG(A2,2))/1000000</f>
+        <f t="shared" ref="F2" si="1">1.6*(A2*LOG(A2,2))/1000000</f>
         <v>1.6383999999999999E-2</v>
       </c>
       <c r="G2" s="10">

</xml_diff>

<commit_message>
Working on assignment 4 anayslis document
</commit_message>
<xml_diff>
--- a/6012/Uploaded Worksheets/assignmentArchive/assignment04 RawData.xlsx
+++ b/6012/Uploaded Worksheets/assignmentArchive/assignment04 RawData.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epoole/Box Sync/erikpoole/6012/Uploaded Worksheets/assignmentArchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6689820A-B7CE-B044-A136-FD86037AC3B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{504FA978-CB75-664E-B706-DAE9005CB41A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="28040" windowHeight="15660" xr2:uid="{E07FD9B9-E6D7-B844-A7A2-A761D0372312}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="28040" windowHeight="15660" activeTab="1" xr2:uid="{E07FD9B9-E6D7-B844-A7A2-A761D0372312}"/>
   </bookViews>
   <sheets>
     <sheet name="QuickSearch - Pivots" sheetId="1" r:id="rId1"/>
+    <sheet name="Quicksort Vs Mergesort" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="22">
   <si>
     <t>Pivot based on Sampling:</t>
   </si>
@@ -55,6 +57,42 @@
   </si>
   <si>
     <t>NLogN</t>
+  </si>
+  <si>
+    <t>Ave.</t>
+  </si>
+  <si>
+    <t>(MergeSort):</t>
+  </si>
+  <si>
+    <t>(Quicksort):</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>(QuickSort):</t>
+  </si>
+  <si>
+    <t>Worst</t>
+  </si>
+  <si>
+    <t>QS Best</t>
+  </si>
+  <si>
+    <t>QS Worst</t>
+  </si>
+  <si>
+    <t>QS Average</t>
+  </si>
+  <si>
+    <t>MS Best</t>
+  </si>
+  <si>
+    <t>MS Average</t>
+  </si>
+  <si>
+    <t>MS Worst</t>
   </si>
 </sst>
 </file>
@@ -114,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -128,6 +166,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -180,7 +222,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>QuickSearch</a:t>
+              <a:t>QuickSort</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1507,6 +1549,1983 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>QuickSort vs. Mergesort</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> n=100</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>QS: Best</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.0558954985499461E-2"/>
+                  <c:y val="1.3733318647235941E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-EB19-E146-A9F4-B58DBC920745}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.9249399999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21615E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.62609E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6439599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2428000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15120140000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32433040000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82425990000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7037827999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.7537175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.8501253999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>QS: Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.4182619839927875E-2"/>
+                  <c:y val="-4.8514014135732288E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-EB19-E146-A9F4-B58DBC920745}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.85445E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2336700000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8790900000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1086429</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2238298</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48976839999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1172683000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7643262000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9152364000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.232437300000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.758324699999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>QS: Worst</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.2725835755416657E-2"/>
+                  <c:y val="-3.0948769148726119E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-EB19-E146-A9F4-B58DBC920745}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.254E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.25729E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.58327E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1758799999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1267200000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15406990000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.31702639999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88623350000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7975757999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.8912784</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.6666392999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>MS: Best</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2043998344141102E-2"/>
+                  <c:y val="3.4625019220975235E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-EB19-E146-A9F4-B58DBC920745}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4.7458500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4745300000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1002812</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8317600000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14686750000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31310909999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71871980000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2085235000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8852608999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.766570099999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.4426749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>MS: Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2043998344141102E-2"/>
+                  <c:y val="-3.4625019220975235E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-EB19-E146-A9F4-B58DBC920745}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.0694799999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1042459</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8738499999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5686099999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14115539999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39008409999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76302239999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2311510000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.7077160999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.197732599999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.879348399999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>MS: Worst</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.418026490041718E-2"/>
+                  <c:y val="6.2325034597755423E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-EB19-E146-A9F4-B58DBC920745}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4.3181999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7915699999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.14717E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4114599999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.142846</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31057410000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66879889999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2261044000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.0103887</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.3229282</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.505770699999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>n</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$H$2:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.1200000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0240000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0480000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0960000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1920000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16384000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32768000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65536000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3107200000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6214400000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.2428800000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>nlog(n)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$I$2:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.1744E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9836799999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5237120000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3013760000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1106559999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15237120000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32505856</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69074944000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4627635200000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0880563199999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.5011711999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>n^2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort'!$J$2:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.4680063999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8720255999999992E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3488102399999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3952409599999988E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7580963839999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15032385535999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60129542143999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4051816857599997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6207267430399988</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.482906972159995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>153.93162788863998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-EB19-E146-A9F4-B58DBC920745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1889495663"/>
+        <c:axId val="1890984927"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1889495663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>ArrayList Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1890984927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1890984927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1889495663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1547,7 +3566,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2104,6 +4679,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10808</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>202391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>50259</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9459</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A5CD133-36EB-7C4F-A233-9C52EA56C7B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2403,8 +5021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6674FF-CCDE-E14E-AC12-71F50906D213}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2459,11 +5077,11 @@
         <v>1.7408E-2</v>
       </c>
       <c r="F2" s="10">
-        <f t="shared" ref="F2" si="1">1.6*(A2*LOG(A2,2))/1000000</f>
+        <f>1.6*(A2*LOG(A2,2))/1000000</f>
         <v>1.6383999999999999E-2</v>
       </c>
       <c r="G2" s="10">
-        <f t="shared" ref="G2:G12" si="2">0.5*(A2*A2)/1000000000</f>
+        <f t="shared" ref="G2:G12" si="1">0.5*(A2*A2)/1000000000</f>
         <v>5.2428800000000003E-4</v>
       </c>
       <c r="L2" s="6">
@@ -2491,11 +5109,11 @@
         <v>3.4816E-2</v>
       </c>
       <c r="F3" s="10">
-        <f t="shared" ref="F3:F11" si="3">1.1*(A3*LOG(A3,2))/1000000</f>
+        <f t="shared" ref="F3:F11" si="2">1.1*(A3*LOG(A3,2))/1000000</f>
         <v>2.4780800000000002E-2</v>
       </c>
       <c r="G3" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.0971520000000001E-3</v>
       </c>
       <c r="L3" s="6">
@@ -2523,11 +5141,11 @@
         <v>6.9631999999999999E-2</v>
       </c>
       <c r="F4" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.4067200000000003E-2</v>
       </c>
       <c r="G4" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8.3886080000000005E-3</v>
       </c>
       <c r="K4" s="1"/>
@@ -2556,11 +5174,11 @@
         <v>0.139264</v>
       </c>
       <c r="F5" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.1171456</v>
       </c>
       <c r="G5" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.3554432000000002E-2</v>
       </c>
       <c r="K5" s="1"/>
@@ -2589,11 +5207,11 @@
         <v>0.278528</v>
       </c>
       <c r="F6" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.25231360000000003</v>
       </c>
       <c r="G6" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.13421772800000001</v>
       </c>
       <c r="K6" s="1"/>
@@ -2655,11 +5273,11 @@
         <v>1.114112</v>
       </c>
       <c r="F8" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.1534336000000001</v>
       </c>
       <c r="G8" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.1474836480000001</v>
       </c>
       <c r="K8" s="1"/>
@@ -2688,11 +5306,11 @@
         <v>2.228224</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.4510464000000005</v>
       </c>
       <c r="G9" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8.5899345920000005</v>
       </c>
       <c r="K9" s="1"/>
@@ -2721,11 +5339,11 @@
         <v>4.456448</v>
       </c>
       <c r="F10" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.1904512</v>
       </c>
       <c r="G10" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>34.359738368000002</v>
       </c>
       <c r="K10" s="1"/>
@@ -2761,11 +5379,11 @@
         <v>8.9128959999999999</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>10.957619200000002</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>137.43895347200001</v>
       </c>
       <c r="K11" s="1"/>
@@ -2805,7 +5423,7 @@
         <v>23.068671999999999</v>
       </c>
       <c r="G12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>549.75581388800003</v>
       </c>
       <c r="L12" s="6">
@@ -3096,4 +5714,1567 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2783969B-5976-2F47-8533-5F7D1B0C1CAC}">
+  <dimension ref="A1:S66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="6">
+        <v>1024</v>
+      </c>
+      <c r="P1" s="6">
+        <v>5.0694799999999998E-2</v>
+      </c>
+      <c r="R1" s="13"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2.9249399999999998E-2</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.85445E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5.254E-3</v>
+      </c>
+      <c r="E2" s="6">
+        <v>4.7458500000000001E-2</v>
+      </c>
+      <c r="F2" s="6">
+        <v>5.0694799999999998E-2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>4.3181999999999998E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" ref="H2:H6" si="0">0.5*(A2)/100000</f>
+        <v>5.1200000000000004E-3</v>
+      </c>
+      <c r="I2" s="10">
+        <f t="shared" ref="I2:I12" si="1">3.1*(A2*LOG(A2,2))/10000000</f>
+        <v>3.1744E-3</v>
+      </c>
+      <c r="J2" s="10">
+        <f t="shared" ref="J2:J12" si="2">1.4*(A2*A2)/10000000000</f>
+        <v>1.4680063999999998E-4</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="6">
+        <v>2048</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0.1042459</v>
+      </c>
+      <c r="R2" s="13"/>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2048</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1.21615E-2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.2336700000000001E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.25729E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>9.4745300000000005E-2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.1042459</v>
+      </c>
+      <c r="G3" s="6">
+        <v>9.7915699999999994E-2</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0240000000000001E-2</v>
+      </c>
+      <c r="I3" s="10">
+        <f t="shared" si="1"/>
+        <v>6.9836799999999999E-3</v>
+      </c>
+      <c r="J3" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8720255999999992E-4</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="6">
+        <v>4096</v>
+      </c>
+      <c r="P3" s="6">
+        <v>8.8738499999999998E-2</v>
+      </c>
+      <c r="R3" s="13"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>4096</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2.62609E-2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>6.8790900000000002E-2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2.58327E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.1002812</v>
+      </c>
+      <c r="F4" s="6">
+        <v>8.8738499999999998E-2</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4.14717E-2</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
+        <v>2.0480000000000002E-2</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5237120000000002E-2</v>
+      </c>
+      <c r="J4" s="10">
+        <f t="shared" si="2"/>
+        <v>2.3488102399999997E-3</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="12">
+        <v>8192</v>
+      </c>
+      <c r="P4" s="12">
+        <v>6.5686099999999997E-2</v>
+      </c>
+      <c r="R4" s="13"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>8192</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5.6439599999999999E-2</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.1086429</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3.1758799999999997E-2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>6.8317600000000006E-2</v>
+      </c>
+      <c r="F5" s="12">
+        <v>6.5686099999999997E-2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>6.4114599999999994E-2</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
+        <v>4.0960000000000003E-2</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" si="1"/>
+        <v>3.3013760000000003E-2</v>
+      </c>
+      <c r="J5" s="10">
+        <f t="shared" si="2"/>
+        <v>9.3952409599999988E-3</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="6">
+        <v>16384</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0.14115539999999999</v>
+      </c>
+      <c r="R5" s="13"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>16384</v>
+      </c>
+      <c r="B6" s="6">
+        <v>7.2428000000000006E-2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.2238298</v>
+      </c>
+      <c r="D6" s="6">
+        <v>7.1267200000000003E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.14686750000000001</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.14115539999999999</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.142846</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>8.1920000000000007E-2</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" si="1"/>
+        <v>7.1106559999999999E-2</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="2"/>
+        <v>3.7580963839999995E-2</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" s="6">
+        <v>32768</v>
+      </c>
+      <c r="P6" s="6">
+        <v>0.39008409999999999</v>
+      </c>
+      <c r="R6" s="13"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>32768</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0.15120140000000001</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.48976839999999999</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.15406990000000001</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.31310909999999997</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.39008409999999999</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0.31057410000000002</v>
+      </c>
+      <c r="H7" s="9">
+        <f>0.5*(A7)/100000</f>
+        <v>0.16384000000000001</v>
+      </c>
+      <c r="I7" s="9">
+        <f>3.1*(A7*LOG(A7,2))/10000000</f>
+        <v>0.15237120000000001</v>
+      </c>
+      <c r="J7" s="9">
+        <f>1.4*(A7*A7)/10000000000</f>
+        <v>0.15032385535999998</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="12">
+        <v>65536</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0.76302239999999999</v>
+      </c>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="15"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>65536</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.32433040000000002</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.1172683000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.31702639999999999</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.71871980000000002</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.76302239999999999</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.66879889999999997</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" ref="H8:H12" si="3">0.5*(A8)/100000</f>
+        <v>0.32768000000000003</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="1"/>
+        <v>0.32505856</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="2"/>
+        <v>0.60129542143999992</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="M8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="6">
+        <v>131072</v>
+      </c>
+      <c r="P8" s="6">
+        <v>3.2311510000000001</v>
+      </c>
+      <c r="R8" s="13"/>
+      <c r="S8" s="4"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>131072</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.82425990000000005</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2.7643262000000002</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.88623350000000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3.2085235000000001</v>
+      </c>
+      <c r="F9" s="6">
+        <v>3.2311510000000001</v>
+      </c>
+      <c r="G9" s="6">
+        <v>3.2261044000000001</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="3"/>
+        <v>0.65536000000000005</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.69074944000000005</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="2"/>
+        <v>2.4051816857599997</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="6">
+        <v>262144</v>
+      </c>
+      <c r="P9" s="6">
+        <v>7.7077160999999998</v>
+      </c>
+      <c r="R9" s="13"/>
+      <c r="S9" s="4"/>
+    </row>
+    <row r="10" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>262144</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.7037827999999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5.9152364000000004</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.7975757999999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6.8852608999999996</v>
+      </c>
+      <c r="F10" s="6">
+        <v>7.7077160999999998</v>
+      </c>
+      <c r="G10" s="6">
+        <v>7.0103887</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="3"/>
+        <v>1.3107200000000001</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="1"/>
+        <v>1.4627635200000002</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="2"/>
+        <v>9.6207267430399988</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="6">
+        <v>524288</v>
+      </c>
+      <c r="P10" s="6">
+        <v>18.197732599999998</v>
+      </c>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="15"/>
+    </row>
+    <row r="11" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>524288</v>
+      </c>
+      <c r="B11" s="6">
+        <v>3.7537175</v>
+      </c>
+      <c r="C11" s="6">
+        <v>15.232437300000001</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3.8912784</v>
+      </c>
+      <c r="E11" s="6">
+        <v>15.766570099999999</v>
+      </c>
+      <c r="F11" s="6">
+        <v>18.197732599999998</v>
+      </c>
+      <c r="G11" s="6">
+        <v>16.3229282</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="3"/>
+        <v>2.6214400000000002</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="1"/>
+        <v>3.0880563199999997</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="2"/>
+        <v>38.482906972159995</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="P11" s="6">
+        <v>42.879348399999998</v>
+      </c>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="15"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="B12" s="6">
+        <v>7.8501253999999996</v>
+      </c>
+      <c r="C12" s="6">
+        <v>31.758324699999999</v>
+      </c>
+      <c r="D12" s="6">
+        <v>8.6666392999999999</v>
+      </c>
+      <c r="E12" s="6">
+        <v>31.4426749</v>
+      </c>
+      <c r="F12" s="6">
+        <v>42.879348399999998</v>
+      </c>
+      <c r="G12" s="6">
+        <v>31.505770699999999</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="3"/>
+        <v>5.2428800000000004</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="1"/>
+        <v>6.5011711999999999</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="2"/>
+        <v>153.93162788863998</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1024</v>
+      </c>
+      <c r="P12" s="6">
+        <v>4.7458500000000001E-2</v>
+      </c>
+      <c r="R12" s="13"/>
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="E13" s="4"/>
+      <c r="M13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="6">
+        <v>2048</v>
+      </c>
+      <c r="P13" s="6">
+        <v>9.4745300000000005E-2</v>
+      </c>
+      <c r="R13" s="13"/>
+      <c r="S13" s="4"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="E14" s="4"/>
+      <c r="M14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" s="6">
+        <v>4096</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0.1002812</v>
+      </c>
+      <c r="R14" s="13"/>
+      <c r="S14" s="4"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="E15" s="4"/>
+      <c r="M15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="6">
+        <v>8192</v>
+      </c>
+      <c r="P15" s="6">
+        <v>6.8317600000000006E-2</v>
+      </c>
+      <c r="R15" s="13"/>
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="C16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="M16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O16" s="6">
+        <v>16384</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0.14686750000000001</v>
+      </c>
+      <c r="R16" s="13"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="M17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="6">
+        <v>32768</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0.31310909999999997</v>
+      </c>
+      <c r="R17" s="13"/>
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="M18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O18" s="6">
+        <v>65536</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0.71871980000000002</v>
+      </c>
+      <c r="R18" s="13"/>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="M19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="6">
+        <v>131072</v>
+      </c>
+      <c r="P19" s="6">
+        <v>3.2085235000000001</v>
+      </c>
+      <c r="R19" s="13"/>
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="M20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O20" s="6">
+        <v>262144</v>
+      </c>
+      <c r="P20" s="6">
+        <v>6.8852608999999996</v>
+      </c>
+      <c r="R20" s="13"/>
+      <c r="S20" s="4"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="M21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O21" s="6">
+        <v>524288</v>
+      </c>
+      <c r="P21" s="6">
+        <v>15.766570099999999</v>
+      </c>
+      <c r="R21" s="13"/>
+      <c r="S21" s="4"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="K22" s="4"/>
+      <c r="M22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="P22" s="6">
+        <v>31.4426749</v>
+      </c>
+      <c r="R22" s="13"/>
+      <c r="S22" s="4"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+      <c r="K23" s="4"/>
+      <c r="M23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="6">
+        <v>1024</v>
+      </c>
+      <c r="P23" s="6">
+        <v>4.3181999999999998E-2</v>
+      </c>
+      <c r="R23" s="13"/>
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="K24" s="4"/>
+      <c r="M24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O24" s="6">
+        <v>2048</v>
+      </c>
+      <c r="P24" s="6">
+        <v>9.7915699999999994E-2</v>
+      </c>
+      <c r="R24" s="13"/>
+      <c r="S24" s="4"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="1"/>
+      <c r="K25" s="4"/>
+      <c r="M25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O25" s="6">
+        <v>4096</v>
+      </c>
+      <c r="P25" s="6">
+        <v>4.14717E-2</v>
+      </c>
+      <c r="R25" s="13"/>
+      <c r="S25" s="4"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="K26" s="4"/>
+      <c r="M26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O26" s="6">
+        <v>8192</v>
+      </c>
+      <c r="P26" s="6">
+        <v>6.4114599999999994E-2</v>
+      </c>
+      <c r="R26" s="13"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="1"/>
+      <c r="K27" s="4"/>
+      <c r="M27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O27" s="6">
+        <v>16384</v>
+      </c>
+      <c r="P27" s="6">
+        <v>0.142846</v>
+      </c>
+      <c r="R27" s="13"/>
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="K28" s="4"/>
+      <c r="M28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O28" s="6">
+        <v>32768</v>
+      </c>
+      <c r="P28" s="6">
+        <v>0.31057410000000002</v>
+      </c>
+      <c r="R28" s="13"/>
+      <c r="S28" s="4"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O29" s="6">
+        <v>65536</v>
+      </c>
+      <c r="P29" s="6">
+        <v>0.66879889999999997</v>
+      </c>
+      <c r="R29" s="13"/>
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="M30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30" s="6">
+        <v>131072</v>
+      </c>
+      <c r="P30" s="6">
+        <v>3.2261044000000001</v>
+      </c>
+      <c r="R30" s="13"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O31" s="6">
+        <v>262144</v>
+      </c>
+      <c r="P31" s="6">
+        <v>7.0103887</v>
+      </c>
+      <c r="R31" s="13"/>
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="M32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O32" s="6">
+        <v>524288</v>
+      </c>
+      <c r="P32" s="6">
+        <v>16.3229282</v>
+      </c>
+      <c r="R32" s="13"/>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O33" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="P33" s="6">
+        <v>31.505770699999999</v>
+      </c>
+      <c r="R33" s="13"/>
+      <c r="S33" s="4"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="M34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" s="6">
+        <v>1024</v>
+      </c>
+      <c r="P34" s="6">
+        <v>2.85445E-2</v>
+      </c>
+      <c r="R34" s="13"/>
+      <c r="S34" s="4"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" s="6">
+        <v>2048</v>
+      </c>
+      <c r="P35" s="6">
+        <v>2.2336700000000001E-2</v>
+      </c>
+      <c r="R35" s="13"/>
+      <c r="S35" s="4"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="M36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" s="6">
+        <v>4096</v>
+      </c>
+      <c r="P36" s="6">
+        <v>6.8790900000000002E-2</v>
+      </c>
+      <c r="R36" s="13"/>
+      <c r="S36" s="4"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="M37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O37" s="6">
+        <v>8192</v>
+      </c>
+      <c r="P37" s="6">
+        <v>0.1086429</v>
+      </c>
+      <c r="R37" s="13"/>
+      <c r="S37" s="4"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="M38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" s="6">
+        <v>16384</v>
+      </c>
+      <c r="P38" s="6">
+        <v>0.2238298</v>
+      </c>
+      <c r="R38" s="13"/>
+      <c r="S38" s="4"/>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="M39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" s="6">
+        <v>32768</v>
+      </c>
+      <c r="P39" s="6">
+        <v>0.48976839999999999</v>
+      </c>
+      <c r="R39" s="13"/>
+      <c r="S39" s="4"/>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+      <c r="M40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O40" s="6">
+        <v>65536</v>
+      </c>
+      <c r="P40" s="6">
+        <v>1.1172683000000001</v>
+      </c>
+      <c r="R40" s="13"/>
+      <c r="S40" s="4"/>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="M41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O41" s="6">
+        <v>131072</v>
+      </c>
+      <c r="P41" s="6">
+        <v>2.7643262000000002</v>
+      </c>
+      <c r="R41" s="13"/>
+      <c r="S41" s="4"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+      <c r="M42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O42" s="6">
+        <v>262144</v>
+      </c>
+      <c r="P42" s="6">
+        <v>5.9152364000000004</v>
+      </c>
+      <c r="R42" s="13"/>
+      <c r="S42" s="4"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="M43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O43" s="6">
+        <v>524288</v>
+      </c>
+      <c r="P43" s="6">
+        <v>15.232437300000001</v>
+      </c>
+      <c r="R43" s="13"/>
+      <c r="S43" s="4"/>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="M44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O44" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="P44" s="6">
+        <v>31.758324699999999</v>
+      </c>
+      <c r="R44" s="13"/>
+      <c r="S44" s="4"/>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="M45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O45" s="6">
+        <v>1024</v>
+      </c>
+      <c r="P45" s="6">
+        <v>2.9249399999999998E-2</v>
+      </c>
+      <c r="R45" s="13"/>
+      <c r="S45" s="4"/>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="M46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O46" s="6">
+        <v>2048</v>
+      </c>
+      <c r="P46" s="6">
+        <v>1.21615E-2</v>
+      </c>
+      <c r="R46" s="13"/>
+      <c r="S46" s="4"/>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="M47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O47" s="6">
+        <v>4096</v>
+      </c>
+      <c r="P47" s="6">
+        <v>2.62609E-2</v>
+      </c>
+      <c r="R47" s="13"/>
+      <c r="S47" s="4"/>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="M48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O48" s="6">
+        <v>8192</v>
+      </c>
+      <c r="P48" s="6">
+        <v>5.6439599999999999E-2</v>
+      </c>
+      <c r="R48" s="13"/>
+      <c r="S48" s="4"/>
+    </row>
+    <row r="49" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O49" s="6">
+        <v>16384</v>
+      </c>
+      <c r="P49" s="6">
+        <v>7.2428000000000006E-2</v>
+      </c>
+      <c r="R49" s="13"/>
+      <c r="S49" s="4"/>
+    </row>
+    <row r="50" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O50" s="6">
+        <v>32768</v>
+      </c>
+      <c r="P50" s="6">
+        <v>0.15120140000000001</v>
+      </c>
+      <c r="R50" s="13"/>
+      <c r="S50" s="4"/>
+    </row>
+    <row r="51" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O51" s="6">
+        <v>65536</v>
+      </c>
+      <c r="P51" s="6">
+        <v>0.32433040000000002</v>
+      </c>
+      <c r="R51" s="13"/>
+      <c r="S51" s="4"/>
+    </row>
+    <row r="52" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O52" s="6">
+        <v>131072</v>
+      </c>
+      <c r="P52" s="6">
+        <v>0.82425990000000005</v>
+      </c>
+      <c r="R52" s="13"/>
+      <c r="S52" s="4"/>
+    </row>
+    <row r="53" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N53" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O53" s="6">
+        <v>262144</v>
+      </c>
+      <c r="P53" s="6">
+        <v>1.7037827999999999</v>
+      </c>
+      <c r="R53" s="13"/>
+      <c r="S53" s="4"/>
+    </row>
+    <row r="54" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O54" s="6">
+        <v>524288</v>
+      </c>
+      <c r="P54" s="6">
+        <v>3.7537175</v>
+      </c>
+      <c r="R54" s="13"/>
+      <c r="S54" s="4"/>
+    </row>
+    <row r="55" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O55" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="P55" s="6">
+        <v>7.8501253999999996</v>
+      </c>
+      <c r="R55" s="13"/>
+      <c r="S55" s="4"/>
+    </row>
+    <row r="56" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O56" s="6">
+        <v>1024</v>
+      </c>
+      <c r="P56" s="6">
+        <v>5.254E-3</v>
+      </c>
+      <c r="R56" s="13"/>
+      <c r="S56" s="4"/>
+    </row>
+    <row r="57" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O57" s="6">
+        <v>2048</v>
+      </c>
+      <c r="P57" s="6">
+        <v>1.25729E-2</v>
+      </c>
+      <c r="R57" s="13"/>
+      <c r="S57" s="4"/>
+    </row>
+    <row r="58" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O58" s="6">
+        <v>4096</v>
+      </c>
+      <c r="P58" s="6">
+        <v>2.58327E-2</v>
+      </c>
+      <c r="R58" s="13"/>
+      <c r="S58" s="4"/>
+    </row>
+    <row r="59" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O59" s="6">
+        <v>8192</v>
+      </c>
+      <c r="P59" s="6">
+        <v>3.1758799999999997E-2</v>
+      </c>
+      <c r="R59" s="13"/>
+      <c r="S59" s="4"/>
+    </row>
+    <row r="60" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O60" s="6">
+        <v>16384</v>
+      </c>
+      <c r="P60" s="6">
+        <v>7.1267200000000003E-2</v>
+      </c>
+      <c r="R60" s="13"/>
+      <c r="S60" s="4"/>
+    </row>
+    <row r="61" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N61" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O61" s="6">
+        <v>32768</v>
+      </c>
+      <c r="P61" s="6">
+        <v>0.15406990000000001</v>
+      </c>
+      <c r="R61" s="13"/>
+      <c r="S61" s="4"/>
+    </row>
+    <row r="62" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O62" s="6">
+        <v>65536</v>
+      </c>
+      <c r="P62" s="6">
+        <v>0.31702639999999999</v>
+      </c>
+      <c r="R62" s="13"/>
+      <c r="S62" s="4"/>
+    </row>
+    <row r="63" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O63" s="6">
+        <v>131072</v>
+      </c>
+      <c r="P63" s="6">
+        <v>0.88623350000000001</v>
+      </c>
+      <c r="R63" s="13"/>
+      <c r="S63" s="4"/>
+    </row>
+    <row r="64" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O64" s="6">
+        <v>262144</v>
+      </c>
+      <c r="P64" s="6">
+        <v>1.7975757999999999</v>
+      </c>
+      <c r="R64" s="13"/>
+      <c r="S64" s="4"/>
+    </row>
+    <row r="65" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O65" s="6">
+        <v>524288</v>
+      </c>
+      <c r="P65" s="6">
+        <v>3.8912784</v>
+      </c>
+      <c r="R65" s="13"/>
+      <c r="S65" s="4"/>
+    </row>
+    <row r="66" spans="13:19" x14ac:dyDescent="0.2">
+      <c r="M66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O66" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="P66" s="6">
+        <v>8.6666392999999999</v>
+      </c>
+      <c r="R66" s="13"/>
+      <c r="S66" s="4"/>
+    </row>
+  </sheetData>
+  <sortState ref="M1:P67">
+    <sortCondition ref="N1:N67"/>
+    <sortCondition ref="M1:M67"/>
+    <sortCondition ref="O1:O67"/>
+  </sortState>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added upload documents for Assignment 4
</commit_message>
<xml_diff>
--- a/6012/Uploaded Worksheets/assignmentArchive/assignment04 RawData.xlsx
+++ b/6012/Uploaded Worksheets/assignmentArchive/assignment04 RawData.xlsx
@@ -8,16 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epoole/Box Sync/erikpoole/6012/Uploaded Worksheets/assignmentArchive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{504FA978-CB75-664E-B706-DAE9005CB41A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D384390-E5AD-2C46-9892-8484E9C6A5B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="28040" windowHeight="15660" activeTab="1" xr2:uid="{E07FD9B9-E6D7-B844-A7A2-A761D0372312}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="28040" windowHeight="15660" activeTab="2" xr2:uid="{E07FD9B9-E6D7-B844-A7A2-A761D0372312}"/>
   </bookViews>
   <sheets>
     <sheet name="QuickSearch - Pivots" sheetId="1" r:id="rId1"/>
     <sheet name="Quicksort Vs Mergesort" sheetId="2" r:id="rId2"/>
+    <sheet name="Quicksort Vs Mergesort (2)" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Quicksort Vs Mergesort (2)'!$A$2:$A$12</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Quicksort Vs Mergesort (2)'!$B$2:$B$12</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Quicksort Vs Mergesort (2)'!$C$2:$C$12</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Quicksort Vs Mergesort (2)'!$D$2:$D$12</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Quicksort Vs Mergesort (2)'!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Quicksort Vs Mergesort (2)'!$F$2:$F$12</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Quicksort Vs Mergesort (2)'!$G$2:$G$12</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Quicksort Vs Mergesort (2)'!$H$2:$H$12</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Quicksort Vs Mergesort (2)'!$I$2:$I$12</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Quicksort Vs Mergesort (2)'!$J$2:$J$12</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="22">
   <si>
     <t>Pivot based on Sampling:</t>
   </si>
@@ -3526,6 +3538,1983 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>QuickSort vs. Mergesort</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> n=1000</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>QS: Best</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.0558954985499461E-2"/>
+                  <c:y val="1.3733318647235941E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-182D-144C-BCB8-F28F9841834F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.6457000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8058999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4807799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5197699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0533899999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15825149999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33073180000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.76709760000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6200671</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5528051</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.4134346000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>QS: Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.4182619839927875E-2"/>
+                  <c:y val="-4.8514014135732288E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-182D-144C-BCB8-F28F9841834F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.6789399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3635699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.36248E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1062813</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23587350000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51802990000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1876770000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6266403999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0597856999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.0209926</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.507513099999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>QS: Worst</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.2725835755416657E-2"/>
+                  <c:y val="-3.0948769148726119E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-182D-144C-BCB8-F28F9841834F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4.1958999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4901000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7451299999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3154100000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4918700000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16277159999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.31910739999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8676005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8456062</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.8800712000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2654140999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>MS: Best</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2043998344141102E-2"/>
+                  <c:y val="3.4625019220975235E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-182D-144C-BCB8-F28F9841834F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.3421499999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.18134E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2582100000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9024800000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1444242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38866689999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78426819999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2697075999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.0635417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.659591000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.556121699999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>MS: Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.2043998344141102E-2"/>
+                  <c:y val="-3.4625019220975235E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-182D-144C-BCB8-F28F9841834F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.54603E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21484E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.82455E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0948700000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1298308</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31776799999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84284210000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2368477000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6065946999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.2636371</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.113109700000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>MS: Worst</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.418026490041718E-2"/>
+                  <c:y val="6.2325034597755423E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-182D-144C-BCB8-F28F9841834F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.30642E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.20719E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.88933E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0079100000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12958030000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28413519999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90502479999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1608881000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8300795000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.636404799999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.698788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>n</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$H$2:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.1200000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0240000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0480000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0960000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1920000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16384000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32768000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65536000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3107200000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6214400000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.2428800000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>nlog(n)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$I$2:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.1744E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9836799999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5237120000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3013760000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1106559999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15237120000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32505856</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69074944000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4627635200000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0880563199999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.5011711999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>n^2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Quicksort Vs Mergesort (2)'!$J$2:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.4680063999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8720255999999992E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3488102399999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3952409599999988E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7580963839999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15032385535999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60129542143999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4051816857599997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6207267430399988</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.482906972159995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>153.93162788863998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-182D-144C-BCB8-F28F9841834F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1889495663"/>
+        <c:axId val="1890984927"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1889495663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>ArrayList Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1890984927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1890984927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1889495663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3567,6 +5556,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4638,6 +6667,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4700,6 +7245,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A5CD133-36EB-7C4F-A233-9C52EA56C7B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>10808</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>202391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>50259</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9459</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356D5E58-52BE-AD4F-9060-60ED72B214A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5720,8 +8308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2783969B-5976-2F47-8533-5F7D1B0C1CAC}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7277,4 +9865,1436 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30695E7E-9E89-124F-82E7-1946EDF210B2}">
+  <dimension ref="A1:Q66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="6"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1">
+        <v>1024</v>
+      </c>
+      <c r="Q1">
+        <v>3.54603E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B2">
+        <v>9.6457000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>1.6789399999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>4.1958999999999998E-3</v>
+      </c>
+      <c r="E2">
+        <v>1.3421499999999999E-2</v>
+      </c>
+      <c r="F2">
+        <v>3.54603E-2</v>
+      </c>
+      <c r="G2">
+        <v>2.30642E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" ref="H2:H6" si="0">0.5*(A2)/100000</f>
+        <v>5.1200000000000004E-3</v>
+      </c>
+      <c r="I2" s="10">
+        <f t="shared" ref="I2:I12" si="1">3.1*(A2*LOG(A2,2))/10000000</f>
+        <v>3.1744E-3</v>
+      </c>
+      <c r="J2" s="10">
+        <f t="shared" ref="J2:J12" si="2">1.4*(A2*A2)/10000000000</f>
+        <v>1.4680063999999998E-4</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>2048</v>
+      </c>
+      <c r="Q2">
+        <v>1.21484E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2048</v>
+      </c>
+      <c r="B3">
+        <v>9.8058999999999993E-3</v>
+      </c>
+      <c r="C3">
+        <v>2.3635699999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>7.4901000000000004E-3</v>
+      </c>
+      <c r="E3">
+        <v>1.18134E-2</v>
+      </c>
+      <c r="F3">
+        <v>1.21484E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.20719E-2</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0240000000000001E-2</v>
+      </c>
+      <c r="I3" s="10">
+        <f t="shared" si="1"/>
+        <v>6.9836799999999999E-3</v>
+      </c>
+      <c r="J3" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8720255999999992E-4</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>4096</v>
+      </c>
+      <c r="Q3">
+        <v>2.82455E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>4096</v>
+      </c>
+      <c r="B4">
+        <v>1.4807799999999999E-2</v>
+      </c>
+      <c r="C4">
+        <v>5.36248E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.7451299999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>3.2582100000000003E-2</v>
+      </c>
+      <c r="F4">
+        <v>2.82455E-2</v>
+      </c>
+      <c r="G4">
+        <v>2.88933E-2</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
+        <v>2.0480000000000002E-2</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5237120000000002E-2</v>
+      </c>
+      <c r="J4" s="10">
+        <f t="shared" si="2"/>
+        <v>2.3488102399999997E-3</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="11">
+        <v>8192</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>6.0948700000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>8192</v>
+      </c>
+      <c r="B5">
+        <v>3.5197699999999998E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.1062813</v>
+      </c>
+      <c r="D5">
+        <v>4.3154100000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>5.9024800000000002E-2</v>
+      </c>
+      <c r="F5" s="11">
+        <v>6.0948700000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>6.0079100000000003E-2</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
+        <v>4.0960000000000003E-2</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" si="1"/>
+        <v>3.3013760000000003E-2</v>
+      </c>
+      <c r="J5" s="10">
+        <f t="shared" si="2"/>
+        <v>9.3952409599999988E-3</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>16384</v>
+      </c>
+      <c r="Q5">
+        <v>0.1298308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>16384</v>
+      </c>
+      <c r="B6">
+        <v>7.0533899999999997E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.23587350000000001</v>
+      </c>
+      <c r="D6">
+        <v>7.4918700000000005E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.1444242</v>
+      </c>
+      <c r="F6">
+        <v>0.1298308</v>
+      </c>
+      <c r="G6">
+        <v>0.12958030000000001</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>8.1920000000000007E-2</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" si="1"/>
+        <v>7.1106559999999999E-2</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="2"/>
+        <v>3.7580963839999995E-2</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="N6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="11">
+        <v>32768</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0.31776799999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>32768</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.15825149999999999</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.51802990000000004</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.16277159999999999</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.38866689999999998</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.31776799999999999</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.28413519999999998</v>
+      </c>
+      <c r="H7" s="10">
+        <f>0.5*(A7)/100000</f>
+        <v>0.16384000000000001</v>
+      </c>
+      <c r="I7" s="10">
+        <f>3.1*(A7*LOG(A7,2))/10000000</f>
+        <v>0.15237120000000001</v>
+      </c>
+      <c r="J7" s="10">
+        <f>1.4*(A7*A7)/10000000000</f>
+        <v>0.15032385535999998</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="11">
+        <v>65536</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0.84284210000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>65536</v>
+      </c>
+      <c r="B8">
+        <v>0.33073180000000002</v>
+      </c>
+      <c r="C8">
+        <v>1.1876770000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.31910739999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.78426819999999997</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.84284210000000004</v>
+      </c>
+      <c r="G8">
+        <v>0.90502479999999996</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" ref="H8:H12" si="3">0.5*(A8)/100000</f>
+        <v>0.32768000000000003</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="1"/>
+        <v>0.32505856</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="2"/>
+        <v>0.60129542143999992</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8">
+        <v>131072</v>
+      </c>
+      <c r="Q8">
+        <v>3.2368477000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>131072</v>
+      </c>
+      <c r="B9">
+        <v>0.76709760000000005</v>
+      </c>
+      <c r="C9">
+        <v>2.6266403999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.8676005</v>
+      </c>
+      <c r="E9">
+        <v>3.2697075999999998</v>
+      </c>
+      <c r="F9">
+        <v>3.2368477000000002</v>
+      </c>
+      <c r="G9">
+        <v>3.1608881000000002</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="3"/>
+        <v>0.65536000000000005</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.69074944000000005</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="2"/>
+        <v>2.4051816857599997</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="N9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9">
+        <v>262144</v>
+      </c>
+      <c r="Q9">
+        <v>7.6065946999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>262144</v>
+      </c>
+      <c r="B10">
+        <v>1.6200671</v>
+      </c>
+      <c r="C10">
+        <v>6.0597856999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.8456062</v>
+      </c>
+      <c r="E10">
+        <v>7.0635417</v>
+      </c>
+      <c r="F10">
+        <v>7.6065946999999996</v>
+      </c>
+      <c r="G10">
+        <v>6.8300795000000001</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="3"/>
+        <v>1.3107200000000001</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="1"/>
+        <v>1.4627635200000002</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="2"/>
+        <v>9.6207267430399988</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10">
+        <v>524288</v>
+      </c>
+      <c r="Q10">
+        <v>18.2636371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>524288</v>
+      </c>
+      <c r="B11">
+        <v>3.5528051</v>
+      </c>
+      <c r="C11">
+        <v>14.0209926</v>
+      </c>
+      <c r="D11">
+        <v>3.8800712000000002</v>
+      </c>
+      <c r="E11">
+        <v>14.659591000000001</v>
+      </c>
+      <c r="F11">
+        <v>18.2636371</v>
+      </c>
+      <c r="G11">
+        <v>14.636404799999999</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="3"/>
+        <v>2.6214400000000002</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="1"/>
+        <v>3.0880563199999997</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="2"/>
+        <v>38.482906972159995</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11">
+        <v>1048576</v>
+      </c>
+      <c r="Q11">
+        <v>40.113109700000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="B12">
+        <v>7.4134346000000004</v>
+      </c>
+      <c r="C12">
+        <v>32.507513099999997</v>
+      </c>
+      <c r="D12">
+        <v>8.2654140999999992</v>
+      </c>
+      <c r="E12">
+        <v>31.556121699999998</v>
+      </c>
+      <c r="F12">
+        <v>40.113109700000003</v>
+      </c>
+      <c r="G12">
+        <v>31.698788</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="3"/>
+        <v>5.2428800000000004</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="1"/>
+        <v>6.5011711999999999</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="2"/>
+        <v>153.93162788863998</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12">
+        <v>1024</v>
+      </c>
+      <c r="Q12">
+        <v>1.3421499999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="E13" s="4"/>
+      <c r="N13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13">
+        <v>2048</v>
+      </c>
+      <c r="Q13">
+        <v>1.18134E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="E14" s="4"/>
+      <c r="N14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14">
+        <v>4096</v>
+      </c>
+      <c r="Q14">
+        <v>3.2582100000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="E15" s="4"/>
+      <c r="N15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O15" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15">
+        <v>8192</v>
+      </c>
+      <c r="Q15">
+        <v>5.9024800000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="C16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="N16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P16">
+        <v>16384</v>
+      </c>
+      <c r="Q16">
+        <v>0.1444242</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="N17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17">
+        <v>32768</v>
+      </c>
+      <c r="Q17">
+        <v>0.38866689999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="N18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18">
+        <v>65536</v>
+      </c>
+      <c r="Q18">
+        <v>0.78426819999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="N19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19">
+        <v>131072</v>
+      </c>
+      <c r="Q19">
+        <v>3.2697075999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="N20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O20" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20">
+        <v>262144</v>
+      </c>
+      <c r="Q20">
+        <v>7.0635417</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="N21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O21" t="s">
+        <v>11</v>
+      </c>
+      <c r="P21">
+        <v>524288</v>
+      </c>
+      <c r="Q21">
+        <v>14.659591000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K22" s="4"/>
+      <c r="N22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O22" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22">
+        <v>1048576</v>
+      </c>
+      <c r="Q22">
+        <v>31.556121699999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+      <c r="K23" s="4"/>
+      <c r="N23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O23" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23">
+        <v>1024</v>
+      </c>
+      <c r="Q23">
+        <v>2.30642E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K24" s="4"/>
+      <c r="N24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O24" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24">
+        <v>2048</v>
+      </c>
+      <c r="Q24">
+        <v>1.20719E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="1"/>
+      <c r="K25" s="4"/>
+      <c r="N25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25" t="s">
+        <v>11</v>
+      </c>
+      <c r="P25">
+        <v>4096</v>
+      </c>
+      <c r="Q25">
+        <v>2.88933E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="K26" s="4"/>
+      <c r="N26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" t="s">
+        <v>11</v>
+      </c>
+      <c r="P26">
+        <v>8192</v>
+      </c>
+      <c r="Q26">
+        <v>6.0079100000000003E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="1"/>
+      <c r="K27" s="4"/>
+      <c r="N27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O27" t="s">
+        <v>11</v>
+      </c>
+      <c r="P27">
+        <v>16384</v>
+      </c>
+      <c r="Q27">
+        <v>0.12958030000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="K28" s="4"/>
+      <c r="N28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O28" t="s">
+        <v>11</v>
+      </c>
+      <c r="P28">
+        <v>32768</v>
+      </c>
+      <c r="Q28">
+        <v>0.28413519999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="1"/>
+      <c r="N29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O29" t="s">
+        <v>11</v>
+      </c>
+      <c r="P29">
+        <v>65536</v>
+      </c>
+      <c r="Q29">
+        <v>0.90502479999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="N30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P30">
+        <v>131072</v>
+      </c>
+      <c r="Q30">
+        <v>3.1608881000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="1"/>
+      <c r="N31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" t="s">
+        <v>11</v>
+      </c>
+      <c r="P31">
+        <v>262144</v>
+      </c>
+      <c r="Q31">
+        <v>6.8300795000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="N32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O32" t="s">
+        <v>11</v>
+      </c>
+      <c r="P32">
+        <v>524288</v>
+      </c>
+      <c r="Q32">
+        <v>14.636404799999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="1"/>
+      <c r="N33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O33" t="s">
+        <v>11</v>
+      </c>
+      <c r="P33">
+        <v>1048576</v>
+      </c>
+      <c r="Q33">
+        <v>31.698788</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="N34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O34" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34">
+        <v>1024</v>
+      </c>
+      <c r="Q34">
+        <v>1.6789399999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="1"/>
+      <c r="N35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35">
+        <v>2048</v>
+      </c>
+      <c r="Q35">
+        <v>2.3635699999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="N36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O36" t="s">
+        <v>12</v>
+      </c>
+      <c r="P36">
+        <v>4096</v>
+      </c>
+      <c r="Q36">
+        <v>5.36248E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="N37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P37">
+        <v>8192</v>
+      </c>
+      <c r="Q37">
+        <v>0.1062813</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="N38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O38" t="s">
+        <v>12</v>
+      </c>
+      <c r="P38">
+        <v>16384</v>
+      </c>
+      <c r="Q38">
+        <v>0.23587350000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="C39" s="3"/>
+      <c r="N39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O39" t="s">
+        <v>12</v>
+      </c>
+      <c r="P39">
+        <v>32768</v>
+      </c>
+      <c r="Q39">
+        <v>0.51802990000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+      <c r="N40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40" t="s">
+        <v>12</v>
+      </c>
+      <c r="P40">
+        <v>65536</v>
+      </c>
+      <c r="Q40">
+        <v>1.1876770000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="3"/>
+      <c r="N41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O41" t="s">
+        <v>12</v>
+      </c>
+      <c r="P41">
+        <v>131072</v>
+      </c>
+      <c r="Q41">
+        <v>2.6266403999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+      <c r="N42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O42" t="s">
+        <v>12</v>
+      </c>
+      <c r="P42">
+        <v>262144</v>
+      </c>
+      <c r="Q42">
+        <v>6.0597856999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O43" t="s">
+        <v>12</v>
+      </c>
+      <c r="P43">
+        <v>524288</v>
+      </c>
+      <c r="Q43">
+        <v>14.0209926</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O44" t="s">
+        <v>12</v>
+      </c>
+      <c r="P44">
+        <v>1048576</v>
+      </c>
+      <c r="Q44">
+        <v>32.507513099999997</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O45" t="s">
+        <v>14</v>
+      </c>
+      <c r="P45">
+        <v>1024</v>
+      </c>
+      <c r="Q45">
+        <v>9.6457000000000001E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O46" t="s">
+        <v>14</v>
+      </c>
+      <c r="P46">
+        <v>2048</v>
+      </c>
+      <c r="Q46">
+        <v>9.8058999999999993E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O47" t="s">
+        <v>14</v>
+      </c>
+      <c r="P47">
+        <v>4096</v>
+      </c>
+      <c r="Q47">
+        <v>1.4807799999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O48" t="s">
+        <v>14</v>
+      </c>
+      <c r="P48">
+        <v>8192</v>
+      </c>
+      <c r="Q48">
+        <v>3.5197699999999998E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O49" t="s">
+        <v>14</v>
+      </c>
+      <c r="P49">
+        <v>16384</v>
+      </c>
+      <c r="Q49">
+        <v>7.0533899999999997E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O50" t="s">
+        <v>14</v>
+      </c>
+      <c r="P50">
+        <v>32768</v>
+      </c>
+      <c r="Q50">
+        <v>0.15825149999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O51" t="s">
+        <v>14</v>
+      </c>
+      <c r="P51">
+        <v>65536</v>
+      </c>
+      <c r="Q51">
+        <v>0.33073180000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O52" t="s">
+        <v>14</v>
+      </c>
+      <c r="P52">
+        <v>131072</v>
+      </c>
+      <c r="Q52">
+        <v>0.76709760000000005</v>
+      </c>
+    </row>
+    <row r="53" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O53" t="s">
+        <v>14</v>
+      </c>
+      <c r="P53">
+        <v>262144</v>
+      </c>
+      <c r="Q53">
+        <v>1.6200671</v>
+      </c>
+    </row>
+    <row r="54" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O54" t="s">
+        <v>14</v>
+      </c>
+      <c r="P54">
+        <v>524288</v>
+      </c>
+      <c r="Q54">
+        <v>3.5528051</v>
+      </c>
+    </row>
+    <row r="55" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O55" t="s">
+        <v>14</v>
+      </c>
+      <c r="P55">
+        <v>1048576</v>
+      </c>
+      <c r="Q55">
+        <v>7.4134346000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O56" t="s">
+        <v>12</v>
+      </c>
+      <c r="P56">
+        <v>1024</v>
+      </c>
+      <c r="Q56">
+        <v>4.1958999999999998E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O57" t="s">
+        <v>12</v>
+      </c>
+      <c r="P57">
+        <v>2048</v>
+      </c>
+      <c r="Q57">
+        <v>7.4901000000000004E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O58" t="s">
+        <v>12</v>
+      </c>
+      <c r="P58">
+        <v>4096</v>
+      </c>
+      <c r="Q58">
+        <v>1.7451299999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O59" t="s">
+        <v>12</v>
+      </c>
+      <c r="P59">
+        <v>8192</v>
+      </c>
+      <c r="Q59">
+        <v>4.3154100000000001E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O60" t="s">
+        <v>12</v>
+      </c>
+      <c r="P60">
+        <v>16384</v>
+      </c>
+      <c r="Q60">
+        <v>7.4918700000000005E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O61" t="s">
+        <v>12</v>
+      </c>
+      <c r="P61">
+        <v>32768</v>
+      </c>
+      <c r="Q61">
+        <v>0.16277159999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O62" t="s">
+        <v>12</v>
+      </c>
+      <c r="P62">
+        <v>65536</v>
+      </c>
+      <c r="Q62">
+        <v>0.31910739999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O63" t="s">
+        <v>12</v>
+      </c>
+      <c r="P63">
+        <v>131072</v>
+      </c>
+      <c r="Q63">
+        <v>0.8676005</v>
+      </c>
+    </row>
+    <row r="64" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O64" t="s">
+        <v>12</v>
+      </c>
+      <c r="P64">
+        <v>262144</v>
+      </c>
+      <c r="Q64">
+        <v>1.8456062</v>
+      </c>
+    </row>
+    <row r="65" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O65" t="s">
+        <v>12</v>
+      </c>
+      <c r="P65">
+        <v>524288</v>
+      </c>
+      <c r="Q65">
+        <v>3.8800712000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="14:17" x14ac:dyDescent="0.2">
+      <c r="N66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O66" t="s">
+        <v>12</v>
+      </c>
+      <c r="P66">
+        <v>1048576</v>
+      </c>
+      <c r="Q66">
+        <v>8.2654140999999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="N1:Q67">
+    <sortCondition ref="O1:O67"/>
+    <sortCondition ref="N1:N67"/>
+    <sortCondition ref="P1:P67"/>
+  </sortState>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>